<commit_message>
My map suggestion (+ some small changes)
</commit_message>
<xml_diff>
--- a/Dataset/AMS_break_ins_per_postal_code.xlsx
+++ b/Dataset/AMS_break_ins_per_postal_code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ear/DS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcalm\DiffeRent_Local\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F26CD504-D104-274E-AFBE-74FD4F35F648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17E1043-3EBA-4325-8981-A9536D643499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{03324705-CD7C-7840-ADD0-1DE88D72ADBD}"/>
+    <workbookView xWindow="3120" yWindow="2400" windowWidth="18828" windowHeight="9312" xr2:uid="{03324705-CD7C-7840-ADD0-1DE88D72ADBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="7">
   <si>
     <t>Postcodegebied</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Poging tot woninginbraak</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -104,7 +110,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -120,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -416,20 +422,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E56C5C6-B691-8242-80D3-0DC93AE7A8CF}">
-  <dimension ref="A1:C230"/>
+  <dimension ref="A1:E230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.296875" customWidth="1"/>
     <col min="2" max="2" width="33.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,8 +445,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1011</v>
       </c>
@@ -450,8 +462,14 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>52.371796000000003</v>
+      </c>
+      <c r="E2">
+        <v>4.9051660000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1011</v>
       </c>
@@ -461,8 +479,14 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>52.371796000000003</v>
+      </c>
+      <c r="E3">
+        <v>4.9051660000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1012</v>
       </c>
@@ -472,8 +496,14 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>52.373809000000001</v>
+      </c>
+      <c r="E4">
+        <v>4.8953420000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1012</v>
       </c>
@@ -483,8 +513,14 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>52.373809000000001</v>
+      </c>
+      <c r="E5">
+        <v>4.8953420000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>1012</v>
       </c>
@@ -494,8 +530,14 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>52.373809000000001</v>
+      </c>
+      <c r="E6">
+        <v>4.8953420000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>1012</v>
       </c>
@@ -505,8 +547,14 @@
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>52.373809000000001</v>
+      </c>
+      <c r="E7">
+        <v>4.8953420000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>1012</v>
       </c>
@@ -516,8 +564,14 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>52.373809000000001</v>
+      </c>
+      <c r="E8">
+        <v>4.8953420000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>1012</v>
       </c>
@@ -527,8 +581,14 @@
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>52.373809000000001</v>
+      </c>
+      <c r="E9">
+        <v>4.8953420000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>1013</v>
       </c>
@@ -538,8 +598,14 @@
       <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E10">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>1013</v>
       </c>
@@ -549,8 +615,14 @@
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E11">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>1013</v>
       </c>
@@ -560,8 +632,14 @@
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E12">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>1013</v>
       </c>
@@ -571,8 +649,14 @@
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E13">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>1013</v>
       </c>
@@ -582,8 +666,14 @@
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E14">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>1013</v>
       </c>
@@ -593,8 +683,14 @@
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E15">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>1013</v>
       </c>
@@ -604,8 +700,14 @@
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E16">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>1013</v>
       </c>
@@ -615,8 +717,14 @@
       <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E17">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>1013</v>
       </c>
@@ -626,8 +734,14 @@
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E18">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>1013</v>
       </c>
@@ -637,8 +751,14 @@
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E19">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>1013</v>
       </c>
@@ -648,8 +768,14 @@
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E20">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>1013</v>
       </c>
@@ -659,8 +785,14 @@
       <c r="C21" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E21">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>1013</v>
       </c>
@@ -670,8 +802,14 @@
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>52.395890000000001</v>
+      </c>
+      <c r="E22">
+        <v>4.8746020000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>1014</v>
       </c>
@@ -681,8 +819,14 @@
       <c r="C23" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>52.391534999999998</v>
+      </c>
+      <c r="E23">
+        <v>4.8606350000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>1014</v>
       </c>
@@ -692,8 +836,14 @@
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>52.391534999999998</v>
+      </c>
+      <c r="E24">
+        <v>4.8606350000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>1014</v>
       </c>
@@ -703,8 +853,14 @@
       <c r="C25" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>52.391534999999998</v>
+      </c>
+      <c r="E25">
+        <v>4.8606350000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>1015</v>
       </c>
@@ -714,8 +870,14 @@
       <c r="C26" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>52.378154000000002</v>
+      </c>
+      <c r="E26">
+        <v>4.8842879999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>1015</v>
       </c>
@@ -725,8 +887,14 @@
       <c r="C27" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>52.378154000000002</v>
+      </c>
+      <c r="E27">
+        <v>4.8842879999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>1015</v>
       </c>
@@ -736,8 +904,14 @@
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>52.378154000000002</v>
+      </c>
+      <c r="E28">
+        <v>4.8842879999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>1016</v>
       </c>
@@ -747,8 +921,14 @@
       <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>52.370911999999997</v>
+      </c>
+      <c r="E29">
+        <v>4.8820699999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>1016</v>
       </c>
@@ -758,8 +938,14 @@
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>52.370911999999997</v>
+      </c>
+      <c r="E30">
+        <v>4.8820699999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>1016</v>
       </c>
@@ -769,8 +955,14 @@
       <c r="C31" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>52.370911999999997</v>
+      </c>
+      <c r="E31">
+        <v>4.8820699999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>1016</v>
       </c>
@@ -780,8 +972,14 @@
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>52.370911999999997</v>
+      </c>
+      <c r="E32">
+        <v>4.8820699999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>1017</v>
       </c>
@@ -791,8 +989,14 @@
       <c r="C33" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>52.362181999999997</v>
+      </c>
+      <c r="E33">
+        <v>4.8934620000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>1017</v>
       </c>
@@ -802,8 +1006,14 @@
       <c r="C34" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>52.362181999999997</v>
+      </c>
+      <c r="E34">
+        <v>4.8934620000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>1017</v>
       </c>
@@ -813,8 +1023,14 @@
       <c r="C35" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>52.362181999999997</v>
+      </c>
+      <c r="E35">
+        <v>4.8934620000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>1018</v>
       </c>
@@ -824,8 +1040,14 @@
       <c r="C36" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E36">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>1018</v>
       </c>
@@ -835,8 +1057,14 @@
       <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E37">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>1018</v>
       </c>
@@ -846,8 +1074,14 @@
       <c r="C38" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E38">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>1018</v>
       </c>
@@ -857,8 +1091,14 @@
       <c r="C39" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E39">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>1018</v>
       </c>
@@ -868,8 +1108,14 @@
       <c r="C40" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E40">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>1018</v>
       </c>
@@ -879,8 +1125,14 @@
       <c r="C41" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E41">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>1018</v>
       </c>
@@ -890,8 +1142,14 @@
       <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E42">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>1018</v>
       </c>
@@ -901,8 +1159,14 @@
       <c r="C43" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E43">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>1018</v>
       </c>
@@ -912,8 +1176,14 @@
       <c r="C44" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E44">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>1018</v>
       </c>
@@ -923,8 +1193,14 @@
       <c r="C45" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E45">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>1018</v>
       </c>
@@ -934,8 +1210,14 @@
       <c r="C46" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>52.367339999999999</v>
+      </c>
+      <c r="E46">
+        <v>4.9176099999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>1019</v>
       </c>
@@ -945,8 +1227,14 @@
       <c r="C47" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>52.373784999999998</v>
+      </c>
+      <c r="E47">
+        <v>4.9304969999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>1019</v>
       </c>
@@ -956,8 +1244,14 @@
       <c r="C48" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>52.373784999999998</v>
+      </c>
+      <c r="E48">
+        <v>4.9304969999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>1019</v>
       </c>
@@ -967,8 +1261,14 @@
       <c r="C49" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>52.373784999999998</v>
+      </c>
+      <c r="E49">
+        <v>4.9304969999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>1019</v>
       </c>
@@ -978,8 +1278,14 @@
       <c r="C50" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>52.373784999999998</v>
+      </c>
+      <c r="E50">
+        <v>4.9304969999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>1019</v>
       </c>
@@ -989,8 +1295,14 @@
       <c r="C51" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>52.373784999999998</v>
+      </c>
+      <c r="E51">
+        <v>4.9304969999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>1022</v>
       </c>
@@ -1000,8 +1312,14 @@
       <c r="C52" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>52.394751999999997</v>
+      </c>
+      <c r="E52">
+        <v>4.9313459999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>1022</v>
       </c>
@@ -1011,8 +1329,14 @@
       <c r="C53" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>52.394751999999997</v>
+      </c>
+      <c r="E53">
+        <v>4.9313459999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>1022</v>
       </c>
@@ -1022,8 +1346,14 @@
       <c r="C54" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>52.394751999999997</v>
+      </c>
+      <c r="E54">
+        <v>4.9313459999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>1023</v>
       </c>
@@ -1033,8 +1363,14 @@
       <c r="C55" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>52.387062999999998</v>
+      </c>
+      <c r="E55">
+        <v>4.9532439999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>1023</v>
       </c>
@@ -1044,8 +1380,14 @@
       <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>52.387062999999998</v>
+      </c>
+      <c r="E56">
+        <v>4.9532439999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>1024</v>
       </c>
@@ -1055,8 +1397,14 @@
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>52.393853999999997</v>
+      </c>
+      <c r="E57">
+        <v>4.9537880000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>1025</v>
       </c>
@@ -1066,8 +1414,14 @@
       <c r="C58" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>52.399410000000003</v>
+      </c>
+      <c r="E58">
+        <v>4.9338100000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>1025</v>
       </c>
@@ -1077,8 +1431,14 @@
       <c r="C59" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>52.399410000000003</v>
+      </c>
+      <c r="E59">
+        <v>4.9338100000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>1025</v>
       </c>
@@ -1088,8 +1448,14 @@
       <c r="C60" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>52.399410000000003</v>
+      </c>
+      <c r="E60">
+        <v>4.9338100000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>1025</v>
       </c>
@@ -1099,8 +1465,14 @@
       <c r="C61" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>52.399410000000003</v>
+      </c>
+      <c r="E61">
+        <v>4.9338100000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>1025</v>
       </c>
@@ -1110,8 +1482,14 @@
       <c r="C62" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>52.399410000000003</v>
+      </c>
+      <c r="E62">
+        <v>4.9338100000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>1025</v>
       </c>
@@ -1121,8 +1499,14 @@
       <c r="C63" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>52.399410000000003</v>
+      </c>
+      <c r="E63">
+        <v>4.9338100000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>1031</v>
       </c>
@@ -1132,8 +1516,14 @@
       <c r="C64" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>52.389252999999997</v>
+      </c>
+      <c r="E64">
+        <v>4.9059270000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>1032</v>
       </c>
@@ -1143,8 +1533,14 @@
       <c r="C65" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>52.397117999999999</v>
+      </c>
+      <c r="E65">
+        <v>4.9113829999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>1032</v>
       </c>
@@ -1154,8 +1550,14 @@
       <c r="C66" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>52.397117999999999</v>
+      </c>
+      <c r="E66">
+        <v>4.9113829999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>1033</v>
       </c>
@@ -1165,8 +1567,14 @@
       <c r="C67" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>52.409871000000003</v>
+      </c>
+      <c r="E67">
+        <v>4.8881629999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>1033</v>
       </c>
@@ -1176,8 +1584,14 @@
       <c r="C68" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>52.409871000000003</v>
+      </c>
+      <c r="E68">
+        <v>4.8881629999999996</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>1034</v>
       </c>
@@ -1187,8 +1601,14 @@
       <c r="C69" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>52.406882000000003</v>
+      </c>
+      <c r="E69">
+        <v>4.915959</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>1034</v>
       </c>
@@ -1198,8 +1618,14 @@
       <c r="C70" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <v>52.406882000000003</v>
+      </c>
+      <c r="E70">
+        <v>4.915959</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>1034</v>
       </c>
@@ -1209,8 +1635,14 @@
       <c r="C71" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>52.406882000000003</v>
+      </c>
+      <c r="E71">
+        <v>4.915959</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>1034</v>
       </c>
@@ -1220,8 +1652,14 @@
       <c r="C72" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>52.406882000000003</v>
+      </c>
+      <c r="E72">
+        <v>4.915959</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>1034</v>
       </c>
@@ -1231,8 +1669,14 @@
       <c r="C73" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <v>52.406882000000003</v>
+      </c>
+      <c r="E73">
+        <v>4.915959</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>1035</v>
       </c>
@@ -1242,8 +1686,14 @@
       <c r="C74" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E74">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>1035</v>
       </c>
@@ -1253,8 +1703,14 @@
       <c r="C75" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E75">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>1035</v>
       </c>
@@ -1264,8 +1720,14 @@
       <c r="C76" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E76">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>1035</v>
       </c>
@@ -1275,8 +1737,14 @@
       <c r="C77" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E77">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>1035</v>
       </c>
@@ -1286,8 +1754,14 @@
       <c r="C78" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E78">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>1035</v>
       </c>
@@ -1297,8 +1771,14 @@
       <c r="C79" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E79">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>1035</v>
       </c>
@@ -1308,8 +1788,14 @@
       <c r="C80" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E80">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>1035</v>
       </c>
@@ -1319,8 +1805,14 @@
       <c r="C81" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E81">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>1035</v>
       </c>
@@ -1330,8 +1822,14 @@
       <c r="C82" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E82">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>1035</v>
       </c>
@@ -1341,8 +1839,14 @@
       <c r="C83" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E83">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>1035</v>
       </c>
@@ -1352,8 +1856,14 @@
       <c r="C84" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E84">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>1035</v>
       </c>
@@ -1363,8 +1873,14 @@
       <c r="C85" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E85">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>1035</v>
       </c>
@@ -1374,8 +1890,14 @@
       <c r="C86" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>52.417679999999997</v>
+      </c>
+      <c r="E86">
+        <v>4.8943349999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>1036</v>
       </c>
@@ -1385,8 +1907,14 @@
       <c r="C87" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <v>52.35295</v>
+      </c>
+      <c r="E87">
+        <v>4.9989039999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>1051</v>
       </c>
@@ -1396,8 +1924,14 @@
       <c r="C88" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <v>52.381051999999997</v>
+      </c>
+      <c r="E88">
+        <v>4.8690290000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>1051</v>
       </c>
@@ -1407,8 +1941,14 @@
       <c r="C89" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <v>52.381051999999997</v>
+      </c>
+      <c r="E89">
+        <v>4.8690290000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>1051</v>
       </c>
@@ -1418,8 +1958,14 @@
       <c r="C90" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <v>52.381051999999997</v>
+      </c>
+      <c r="E90">
+        <v>4.8690290000000003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>1051</v>
       </c>
@@ -1429,8 +1975,14 @@
       <c r="C91" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <v>52.381051999999997</v>
+      </c>
+      <c r="E91">
+        <v>4.8690290000000003</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>1051</v>
       </c>
@@ -1440,8 +1992,14 @@
       <c r="C92" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D92">
+        <v>52.381051999999997</v>
+      </c>
+      <c r="E92">
+        <v>4.8690290000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>1051</v>
       </c>
@@ -1451,8 +2009,14 @@
       <c r="C93" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D93">
+        <v>52.381051999999997</v>
+      </c>
+      <c r="E93">
+        <v>4.8690290000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>1051</v>
       </c>
@@ -1462,8 +2026,14 @@
       <c r="C94" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D94">
+        <v>52.381051999999997</v>
+      </c>
+      <c r="E94">
+        <v>4.8690290000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>1052</v>
       </c>
@@ -1473,8 +2043,14 @@
       <c r="C95" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <v>52.376904000000003</v>
+      </c>
+      <c r="E95">
+        <v>4.8739939999999997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>1052</v>
       </c>
@@ -1484,8 +2060,14 @@
       <c r="C96" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D96">
+        <v>52.376904000000003</v>
+      </c>
+      <c r="E96">
+        <v>4.8739939999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>1053</v>
       </c>
@@ -1495,8 +2077,14 @@
       <c r="C97" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D97">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E97">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>1053</v>
       </c>
@@ -1506,8 +2094,14 @@
       <c r="C98" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D98">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E98">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>1053</v>
       </c>
@@ -1517,8 +2111,14 @@
       <c r="C99" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D99">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E99">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>1053</v>
       </c>
@@ -1528,8 +2128,14 @@
       <c r="C100" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E100">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>1053</v>
       </c>
@@ -1539,8 +2145,14 @@
       <c r="C101" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D101">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E101">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>1053</v>
       </c>
@@ -1550,8 +2162,14 @@
       <c r="C102" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D102">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E102">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>1053</v>
       </c>
@@ -1561,8 +2179,14 @@
       <c r="C103" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D103">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E103">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>1053</v>
       </c>
@@ -1572,8 +2196,14 @@
       <c r="C104" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D104">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E104">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>1053</v>
       </c>
@@ -1583,8 +2213,14 @@
       <c r="C105" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D105">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E105">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>1053</v>
       </c>
@@ -1594,8 +2230,14 @@
       <c r="C106" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D106">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E106">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>1053</v>
       </c>
@@ -1605,8 +2247,14 @@
       <c r="C107" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D107">
+        <v>52.367001999999999</v>
+      </c>
+      <c r="E107">
+        <v>4.8683129999999997</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>1054</v>
       </c>
@@ -1616,8 +2264,14 @@
       <c r="C108" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D108">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E108">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>1054</v>
       </c>
@@ -1627,8 +2281,14 @@
       <c r="C109" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D109">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E109">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>1054</v>
       </c>
@@ -1638,8 +2298,14 @@
       <c r="C110" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D110">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E110">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>1054</v>
       </c>
@@ -1649,8 +2315,14 @@
       <c r="C111" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D111">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E111">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>1054</v>
       </c>
@@ -1660,8 +2332,14 @@
       <c r="C112" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D112">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E112">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>1054</v>
       </c>
@@ -1671,8 +2349,14 @@
       <c r="C113" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D113">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E113">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>1054</v>
       </c>
@@ -1682,8 +2366,14 @@
       <c r="C114" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D114">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E114">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>1054</v>
       </c>
@@ -1693,8 +2383,14 @@
       <c r="C115" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D115">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E115">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>1054</v>
       </c>
@@ -1704,8 +2400,14 @@
       <c r="C116" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D116">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E116">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A117" s="2">
         <v>1054</v>
       </c>
@@ -1715,8 +2417,14 @@
       <c r="C117" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D117">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E117">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A118" s="2">
         <v>1054</v>
       </c>
@@ -1726,8 +2434,14 @@
       <c r="C118" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D118">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E118">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A119" s="2">
         <v>1054</v>
       </c>
@@ -1737,8 +2451,14 @@
       <c r="C119" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D119">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E119">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A120" s="2">
         <v>1054</v>
       </c>
@@ -1748,8 +2468,14 @@
       <c r="C120" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D120">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E120">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>1054</v>
       </c>
@@ -1759,8 +2485,14 @@
       <c r="C121" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D121">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E121">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>1054</v>
       </c>
@@ -1770,8 +2502,14 @@
       <c r="C122" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D122">
+        <v>52.361542999999998</v>
+      </c>
+      <c r="E122">
+        <v>4.8684079999999996</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>1055</v>
       </c>
@@ -1781,8 +2519,14 @@
       <c r="C123" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D123">
+        <v>52.380377000000003</v>
+      </c>
+      <c r="E123">
+        <v>4.8527699999999996</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>1055</v>
       </c>
@@ -1792,8 +2536,14 @@
       <c r="C124" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D124">
+        <v>52.380377000000003</v>
+      </c>
+      <c r="E124">
+        <v>4.8527699999999996</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>1055</v>
       </c>
@@ -1803,8 +2553,14 @@
       <c r="C125" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D125">
+        <v>52.380377000000003</v>
+      </c>
+      <c r="E125">
+        <v>4.8527699999999996</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>1056</v>
       </c>
@@ -1814,8 +2570,14 @@
       <c r="C126" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D126">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E126">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>1056</v>
       </c>
@@ -1825,8 +2587,14 @@
       <c r="C127" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D127">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E127">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>1056</v>
       </c>
@@ -1836,8 +2604,14 @@
       <c r="C128" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D128">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E128">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A129" s="2">
         <v>1056</v>
       </c>
@@ -1847,8 +2621,14 @@
       <c r="C129" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D129">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E129">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>1056</v>
       </c>
@@ -1858,8 +2638,14 @@
       <c r="C130" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D130">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E130">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>1056</v>
       </c>
@@ -1869,8 +2655,14 @@
       <c r="C131" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D131">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E131">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A132" s="2">
         <v>1056</v>
       </c>
@@ -1880,8 +2672,14 @@
       <c r="C132" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D132">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E132">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A133" s="2">
         <v>1056</v>
       </c>
@@ -1891,8 +2689,14 @@
       <c r="C133" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D133">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E133">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>1056</v>
       </c>
@@ -1902,8 +2706,14 @@
       <c r="C134" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D134">
+        <v>52.373260999999999</v>
+      </c>
+      <c r="E134">
+        <v>4.854285</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>1057</v>
       </c>
@@ -1913,8 +2723,14 @@
       <c r="C135" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D135">
+        <v>52.367438</v>
+      </c>
+      <c r="E135">
+        <v>4.8534740000000003</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>1057</v>
       </c>
@@ -1924,8 +2740,14 @@
       <c r="C136" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D136">
+        <v>52.367438</v>
+      </c>
+      <c r="E136">
+        <v>4.8534740000000003</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>1057</v>
       </c>
@@ -1935,8 +2757,14 @@
       <c r="C137" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D137">
+        <v>52.367438</v>
+      </c>
+      <c r="E137">
+        <v>4.8534740000000003</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>1057</v>
       </c>
@@ -1946,8 +2774,14 @@
       <c r="C138" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D138">
+        <v>52.367438</v>
+      </c>
+      <c r="E138">
+        <v>4.8534740000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>1058</v>
       </c>
@@ -1957,8 +2791,14 @@
       <c r="C139" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D139">
+        <v>52.358117999999997</v>
+      </c>
+      <c r="E139">
+        <v>4.8490609999999998</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A140" s="2">
         <v>1058</v>
       </c>
@@ -1968,8 +2808,14 @@
       <c r="C140" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D140">
+        <v>52.358117999999997</v>
+      </c>
+      <c r="E140">
+        <v>4.8490609999999998</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A141" s="2">
         <v>1058</v>
       </c>
@@ -1979,8 +2825,14 @@
       <c r="C141" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D141">
+        <v>52.358117999999997</v>
+      </c>
+      <c r="E141">
+        <v>4.8490609999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A142" s="2">
         <v>1058</v>
       </c>
@@ -1990,8 +2842,14 @@
       <c r="C142" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D142">
+        <v>52.358117999999997</v>
+      </c>
+      <c r="E142">
+        <v>4.8490609999999998</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>1058</v>
       </c>
@@ -2001,8 +2859,14 @@
       <c r="C143" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D143">
+        <v>52.358117999999997</v>
+      </c>
+      <c r="E143">
+        <v>4.8490609999999998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>1058</v>
       </c>
@@ -2012,8 +2876,14 @@
       <c r="C144" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D144">
+        <v>52.358117999999997</v>
+      </c>
+      <c r="E144">
+        <v>4.8490609999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>1058</v>
       </c>
@@ -2023,8 +2893,14 @@
       <c r="C145" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D145">
+        <v>52.358117999999997</v>
+      </c>
+      <c r="E145">
+        <v>4.8490609999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A146" s="2">
         <v>1059</v>
       </c>
@@ -2034,8 +2910,14 @@
       <c r="C146" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D146">
+        <v>52.345745999999998</v>
+      </c>
+      <c r="E146">
+        <v>4.8461040000000004</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A147" s="2">
         <v>1059</v>
       </c>
@@ -2045,8 +2927,14 @@
       <c r="C147" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D147">
+        <v>52.345745999999998</v>
+      </c>
+      <c r="E147">
+        <v>4.8461040000000004</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A148" s="2">
         <v>1059</v>
       </c>
@@ -2056,8 +2944,14 @@
       <c r="C148" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D148">
+        <v>52.345745999999998</v>
+      </c>
+      <c r="E148">
+        <v>4.8461040000000004</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A149" s="2">
         <v>1059</v>
       </c>
@@ -2067,8 +2961,14 @@
       <c r="C149" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D149">
+        <v>52.345745999999998</v>
+      </c>
+      <c r="E149">
+        <v>4.8461040000000004</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A150" s="2">
         <v>1059</v>
       </c>
@@ -2078,8 +2978,14 @@
       <c r="C150" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D150">
+        <v>52.345745999999998</v>
+      </c>
+      <c r="E150">
+        <v>4.8461040000000004</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A151" s="2">
         <v>1059</v>
       </c>
@@ -2089,8 +2995,14 @@
       <c r="C151" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D151">
+        <v>52.345745999999998</v>
+      </c>
+      <c r="E151">
+        <v>4.8461040000000004</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A152" s="2">
         <v>1059</v>
       </c>
@@ -2100,8 +3012,14 @@
       <c r="C152" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D152">
+        <v>52.345745999999998</v>
+      </c>
+      <c r="E152">
+        <v>4.8461040000000004</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A153" s="2">
         <v>1059</v>
       </c>
@@ -2111,8 +3029,14 @@
       <c r="C153" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D153">
+        <v>52.345745999999998</v>
+      </c>
+      <c r="E153">
+        <v>4.8461040000000004</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A154" s="2">
         <v>1061</v>
       </c>
@@ -2122,8 +3046,14 @@
       <c r="C154" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D154">
+        <v>52.373182999999997</v>
+      </c>
+      <c r="E154">
+        <v>4.8397420000000002</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A155" s="2">
         <v>1061</v>
       </c>
@@ -2133,8 +3063,14 @@
       <c r="C155" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D155">
+        <v>52.373182999999997</v>
+      </c>
+      <c r="E155">
+        <v>4.8397420000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A156" s="2">
         <v>1071</v>
       </c>
@@ -2144,8 +3080,14 @@
       <c r="C156" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D156">
+        <v>52.356195999999997</v>
+      </c>
+      <c r="E156">
+        <v>4.8775409999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A157" s="2">
         <v>1071</v>
       </c>
@@ -2155,8 +3097,14 @@
       <c r="C157" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D157">
+        <v>52.356195999999997</v>
+      </c>
+      <c r="E157">
+        <v>4.8775409999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A158" s="2">
         <v>1071</v>
       </c>
@@ -2166,8 +3114,14 @@
       <c r="C158" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D158">
+        <v>52.356195999999997</v>
+      </c>
+      <c r="E158">
+        <v>4.8775409999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A159" s="2">
         <v>1072</v>
       </c>
@@ -2177,8 +3131,14 @@
       <c r="C159" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D159">
+        <v>52.353448</v>
+      </c>
+      <c r="E159">
+        <v>4.8915240000000004</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A160" s="2">
         <v>1072</v>
       </c>
@@ -2188,8 +3148,14 @@
       <c r="C160" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D160">
+        <v>52.353448</v>
+      </c>
+      <c r="E160">
+        <v>4.8915240000000004</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A161" s="2">
         <v>1072</v>
       </c>
@@ -2199,8 +3165,14 @@
       <c r="C161" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D161">
+        <v>52.353448</v>
+      </c>
+      <c r="E161">
+        <v>4.8915240000000004</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A162" s="2">
         <v>1072</v>
       </c>
@@ -2210,8 +3182,14 @@
       <c r="C162" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D162">
+        <v>52.353448</v>
+      </c>
+      <c r="E162">
+        <v>4.8915240000000004</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A163" s="2">
         <v>1072</v>
       </c>
@@ -2221,8 +3199,14 @@
       <c r="C163" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D163">
+        <v>52.353448</v>
+      </c>
+      <c r="E163">
+        <v>4.8915240000000004</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A164" s="2">
         <v>1073</v>
       </c>
@@ -2232,8 +3216,14 @@
       <c r="C164" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D164">
+        <v>52.353144</v>
+      </c>
+      <c r="E164">
+        <v>4.8979309999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A165" s="2">
         <v>1073</v>
       </c>
@@ -2243,8 +3233,14 @@
       <c r="C165" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D165">
+        <v>52.353144</v>
+      </c>
+      <c r="E165">
+        <v>4.8979309999999998</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A166" s="2">
         <v>1073</v>
       </c>
@@ -2254,8 +3250,14 @@
       <c r="C166" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D166">
+        <v>52.353144</v>
+      </c>
+      <c r="E166">
+        <v>4.8979309999999998</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A167" s="2">
         <v>1073</v>
       </c>
@@ -2265,8 +3267,14 @@
       <c r="C167" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D167">
+        <v>52.353144</v>
+      </c>
+      <c r="E167">
+        <v>4.8979309999999998</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A168" s="2">
         <v>1073</v>
       </c>
@@ -2276,8 +3284,14 @@
       <c r="C168" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D168">
+        <v>52.353144</v>
+      </c>
+      <c r="E168">
+        <v>4.8979309999999998</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A169" s="2">
         <v>1073</v>
       </c>
@@ -2287,8 +3301,14 @@
       <c r="C169" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D169">
+        <v>52.353144</v>
+      </c>
+      <c r="E169">
+        <v>4.8979309999999998</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A170" s="2">
         <v>1073</v>
       </c>
@@ -2298,8 +3318,14 @@
       <c r="C170" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D170">
+        <v>52.353144</v>
+      </c>
+      <c r="E170">
+        <v>4.8979309999999998</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A171" s="2">
         <v>1074</v>
       </c>
@@ -2309,8 +3335,14 @@
       <c r="C171" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D171">
+        <v>52.353839999999998</v>
+      </c>
+      <c r="E171">
+        <v>4.9046500000000002</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A172" s="2">
         <v>1074</v>
       </c>
@@ -2320,8 +3352,14 @@
       <c r="C172" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D172">
+        <v>52.353839999999998</v>
+      </c>
+      <c r="E172">
+        <v>4.9046500000000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A173" s="2">
         <v>1074</v>
       </c>
@@ -2331,8 +3369,14 @@
       <c r="C173" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D173">
+        <v>52.353839999999998</v>
+      </c>
+      <c r="E173">
+        <v>4.9046500000000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A174" s="2">
         <v>1075</v>
       </c>
@@ -2342,8 +3386,14 @@
       <c r="C174" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D174">
+        <v>52.068030999999998</v>
+      </c>
+      <c r="E174">
+        <v>4.2731120000000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A175" s="2">
         <v>1075</v>
       </c>
@@ -2353,8 +3403,14 @@
       <c r="C175" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D175">
+        <v>52.068030999999998</v>
+      </c>
+      <c r="E175">
+        <v>4.2731120000000002</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A176" s="2">
         <v>1075</v>
       </c>
@@ -2364,8 +3420,14 @@
       <c r="C176" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D176">
+        <v>52.068030999999998</v>
+      </c>
+      <c r="E176">
+        <v>4.2731120000000002</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A177" s="2">
         <v>1075</v>
       </c>
@@ -2375,8 +3437,14 @@
       <c r="C177" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D177">
+        <v>52.068030999999998</v>
+      </c>
+      <c r="E177">
+        <v>4.2731120000000002</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A178" s="2">
         <v>1075</v>
       </c>
@@ -2386,8 +3454,14 @@
       <c r="C178" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D178">
+        <v>52.068030999999998</v>
+      </c>
+      <c r="E178">
+        <v>4.2731120000000002</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A179" s="2">
         <v>1076</v>
       </c>
@@ -2397,8 +3471,14 @@
       <c r="C179" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D179">
+        <v>52.343513000000002</v>
+      </c>
+      <c r="E179">
+        <v>4.8584110000000003</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A180" s="2">
         <v>1076</v>
       </c>
@@ -2408,8 +3488,14 @@
       <c r="C180" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D180">
+        <v>52.343513000000002</v>
+      </c>
+      <c r="E180">
+        <v>4.8584110000000003</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A181" s="2">
         <v>1076</v>
       </c>
@@ -2419,8 +3505,14 @@
       <c r="C181" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D181">
+        <v>52.343513000000002</v>
+      </c>
+      <c r="E181">
+        <v>4.8584110000000003</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A182" s="2">
         <v>1076</v>
       </c>
@@ -2430,8 +3522,14 @@
       <c r="C182" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D182">
+        <v>52.343513000000002</v>
+      </c>
+      <c r="E182">
+        <v>4.8584110000000003</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A183" s="2">
         <v>1076</v>
       </c>
@@ -2441,8 +3539,14 @@
       <c r="C183" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D183">
+        <v>52.343513000000002</v>
+      </c>
+      <c r="E183">
+        <v>4.8584110000000003</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A184" s="2">
         <v>1076</v>
       </c>
@@ -2452,8 +3556,14 @@
       <c r="C184" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D184">
+        <v>52.343513000000002</v>
+      </c>
+      <c r="E184">
+        <v>4.8584110000000003</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A185" s="2">
         <v>1076</v>
       </c>
@@ -2463,8 +3573,14 @@
       <c r="C185" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D185">
+        <v>52.343513000000002</v>
+      </c>
+      <c r="E185">
+        <v>4.8584110000000003</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A186" s="2">
         <v>1077</v>
       </c>
@@ -2474,8 +3590,14 @@
       <c r="C186" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D186">
+        <v>52.316240000000001</v>
+      </c>
+      <c r="E186">
+        <v>4.9814790000000002</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A187" s="2">
         <v>1077</v>
       </c>
@@ -2485,8 +3607,14 @@
       <c r="C187" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D187">
+        <v>52.316240000000001</v>
+      </c>
+      <c r="E187">
+        <v>4.9814790000000002</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A188" s="2">
         <v>1077</v>
       </c>
@@ -2496,8 +3624,14 @@
       <c r="C188" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D188">
+        <v>52.316240000000001</v>
+      </c>
+      <c r="E188">
+        <v>4.9814790000000002</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A189" s="2">
         <v>1077</v>
       </c>
@@ -2507,8 +3641,14 @@
       <c r="C189" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D189">
+        <v>52.316240000000001</v>
+      </c>
+      <c r="E189">
+        <v>4.9814790000000002</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A190" s="2">
         <v>1077</v>
       </c>
@@ -2518,8 +3658,14 @@
       <c r="C190" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D190">
+        <v>52.316240000000001</v>
+      </c>
+      <c r="E190">
+        <v>4.9814790000000002</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A191" s="2">
         <v>1077</v>
       </c>
@@ -2529,8 +3675,14 @@
       <c r="C191" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D191">
+        <v>52.316240000000001</v>
+      </c>
+      <c r="E191">
+        <v>4.9814790000000002</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A192" s="2">
         <v>1078</v>
       </c>
@@ -2540,8 +3692,14 @@
       <c r="C192" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D192">
+        <v>52.345039</v>
+      </c>
+      <c r="E192">
+        <v>4.896458</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A193" s="2">
         <v>1078</v>
       </c>
@@ -2551,8 +3709,14 @@
       <c r="C193" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D193">
+        <v>52.345039</v>
+      </c>
+      <c r="E193">
+        <v>4.896458</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A194" s="2">
         <v>1078</v>
       </c>
@@ -2562,8 +3726,14 @@
       <c r="C194" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D194">
+        <v>52.345039</v>
+      </c>
+      <c r="E194">
+        <v>4.896458</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A195" s="2">
         <v>1078</v>
       </c>
@@ -2573,8 +3743,14 @@
       <c r="C195" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D195">
+        <v>52.345039</v>
+      </c>
+      <c r="E195">
+        <v>4.896458</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A196" s="2">
         <v>1078</v>
       </c>
@@ -2584,8 +3760,14 @@
       <c r="C196" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D196">
+        <v>52.345039</v>
+      </c>
+      <c r="E196">
+        <v>4.896458</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A197" s="2">
         <v>1079</v>
       </c>
@@ -2595,8 +3777,14 @@
       <c r="C197" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D197">
+        <v>52.340465000000002</v>
+      </c>
+      <c r="E197">
+        <v>4.9037329999999999</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A198" s="2">
         <v>1079</v>
       </c>
@@ -2606,8 +3794,14 @@
       <c r="C198" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D198">
+        <v>52.340465000000002</v>
+      </c>
+      <c r="E198">
+        <v>4.9037329999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A199" s="2">
         <v>1079</v>
       </c>
@@ -2617,8 +3811,14 @@
       <c r="C199" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D199">
+        <v>52.340465000000002</v>
+      </c>
+      <c r="E199">
+        <v>4.9037329999999999</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A200" s="2">
         <v>1079</v>
       </c>
@@ -2628,8 +3828,14 @@
       <c r="C200" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D200">
+        <v>52.340465000000002</v>
+      </c>
+      <c r="E200">
+        <v>4.9037329999999999</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A201" s="2">
         <v>1079</v>
       </c>
@@ -2639,8 +3845,14 @@
       <c r="C201" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D201">
+        <v>52.340465000000002</v>
+      </c>
+      <c r="E201">
+        <v>4.9037329999999999</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A202" s="2">
         <v>1079</v>
       </c>
@@ -2650,8 +3862,14 @@
       <c r="C202" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D202">
+        <v>52.340465000000002</v>
+      </c>
+      <c r="E202">
+        <v>4.9037329999999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A203" s="2">
         <v>1082</v>
       </c>
@@ -2661,8 +3879,14 @@
       <c r="C203" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D203">
+        <v>52.330398000000002</v>
+      </c>
+      <c r="E203">
+        <v>4.8749719999999996</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A204" s="2">
         <v>1082</v>
       </c>
@@ -2672,8 +3896,14 @@
       <c r="C204" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D204">
+        <v>52.330398000000002</v>
+      </c>
+      <c r="E204">
+        <v>4.8749719999999996</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A205" s="2">
         <v>1091</v>
       </c>
@@ -2683,8 +3913,14 @@
       <c r="C205" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D205">
+        <v>52.355322000000001</v>
+      </c>
+      <c r="E205">
+        <v>4.9132930000000004</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A206" s="2">
         <v>1091</v>
       </c>
@@ -2694,8 +3930,14 @@
       <c r="C206" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D206">
+        <v>52.355322000000001</v>
+      </c>
+      <c r="E206">
+        <v>4.9132930000000004</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A207" s="2">
         <v>1091</v>
       </c>
@@ -2705,8 +3947,14 @@
       <c r="C207" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D207">
+        <v>52.355322000000001</v>
+      </c>
+      <c r="E207">
+        <v>4.9132930000000004</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A208" s="2">
         <v>1091</v>
       </c>
@@ -2716,8 +3964,14 @@
       <c r="C208" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D208">
+        <v>52.355322000000001</v>
+      </c>
+      <c r="E208">
+        <v>4.9132930000000004</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A209" s="2">
         <v>1091</v>
       </c>
@@ -2727,8 +3981,14 @@
       <c r="C209" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D209">
+        <v>52.355322000000001</v>
+      </c>
+      <c r="E209">
+        <v>4.9132930000000004</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A210" s="2">
         <v>1092</v>
       </c>
@@ -2738,8 +3998,14 @@
       <c r="C210" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D210">
+        <v>52.358325999999998</v>
+      </c>
+      <c r="E210">
+        <v>4.9218260000000003</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A211" s="2">
         <v>1092</v>
       </c>
@@ -2749,8 +4015,14 @@
       <c r="C211" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D211">
+        <v>52.358325999999998</v>
+      </c>
+      <c r="E211">
+        <v>4.9218260000000003</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A212" s="2">
         <v>1093</v>
       </c>
@@ -2760,8 +4032,14 @@
       <c r="C212" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D212">
+        <v>52.361055</v>
+      </c>
+      <c r="E212">
+        <v>4.9293779999999998</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A213" s="2">
         <v>1093</v>
       </c>
@@ -2771,8 +4049,14 @@
       <c r="C213" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D213">
+        <v>52.361055</v>
+      </c>
+      <c r="E213">
+        <v>4.9293779999999998</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A214" s="2">
         <v>1093</v>
       </c>
@@ -2782,8 +4066,14 @@
       <c r="C214" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D214">
+        <v>52.361055</v>
+      </c>
+      <c r="E214">
+        <v>4.9293779999999998</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A215" s="2">
         <v>1093</v>
       </c>
@@ -2793,8 +4083,14 @@
       <c r="C215" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D215">
+        <v>52.361055</v>
+      </c>
+      <c r="E215">
+        <v>4.9293779999999998</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A216" s="2">
         <v>1094</v>
       </c>
@@ -2804,8 +4100,14 @@
       <c r="C216" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D216">
+        <v>52.362485999999997</v>
+      </c>
+      <c r="E216">
+        <v>4.9362300000000001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A217" s="2">
         <v>1094</v>
       </c>
@@ -2815,8 +4117,14 @@
       <c r="C217" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D217">
+        <v>52.362485999999997</v>
+      </c>
+      <c r="E217">
+        <v>4.9362300000000001</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A218" s="2">
         <v>1094</v>
       </c>
@@ -2826,8 +4134,14 @@
       <c r="C218" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D218">
+        <v>52.362485999999997</v>
+      </c>
+      <c r="E218">
+        <v>4.9362300000000001</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A219" s="2">
         <v>1095</v>
       </c>
@@ -2837,8 +4151,14 @@
       <c r="C219" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D219">
+        <v>52.360709</v>
+      </c>
+      <c r="E219">
+        <v>4.9703980000000003</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A220" s="2">
         <v>1096</v>
       </c>
@@ -2848,8 +4168,14 @@
       <c r="C220" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D220">
+        <v>52.333452999999999</v>
+      </c>
+      <c r="E220">
+        <v>4.9145060000000003</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A221" s="2">
         <v>1096</v>
       </c>
@@ -2859,8 +4185,14 @@
       <c r="C221" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D221">
+        <v>52.333452999999999</v>
+      </c>
+      <c r="E221">
+        <v>4.9145060000000003</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A222" s="2">
         <v>1096</v>
       </c>
@@ -2870,8 +4202,14 @@
       <c r="C222" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D222">
+        <v>52.333452999999999</v>
+      </c>
+      <c r="E222">
+        <v>4.9145060000000003</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A223" s="2">
         <v>1097</v>
       </c>
@@ -2881,8 +4219,14 @@
       <c r="C223" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D223">
+        <v>52.345621999999999</v>
+      </c>
+      <c r="E223">
+        <v>4.9310489999999998</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A224" s="2">
         <v>1097</v>
       </c>
@@ -2892,8 +4236,14 @@
       <c r="C224" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D224">
+        <v>52.345621999999999</v>
+      </c>
+      <c r="E224">
+        <v>4.9310489999999998</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A225" s="2">
         <v>1097</v>
       </c>
@@ -2903,8 +4253,14 @@
       <c r="C225" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D225">
+        <v>52.345621999999999</v>
+      </c>
+      <c r="E225">
+        <v>4.9310489999999998</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A226" s="2">
         <v>1097</v>
       </c>
@@ -2914,8 +4270,14 @@
       <c r="C226" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D226">
+        <v>52.345621999999999</v>
+      </c>
+      <c r="E226">
+        <v>4.9310489999999998</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A227" s="2">
         <v>1097</v>
       </c>
@@ -2925,8 +4287,14 @@
       <c r="C227" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D227">
+        <v>52.345621999999999</v>
+      </c>
+      <c r="E227">
+        <v>4.9310489999999998</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A228" s="2">
         <v>1097</v>
       </c>
@@ -2936,8 +4304,14 @@
       <c r="C228" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D228">
+        <v>52.345621999999999</v>
+      </c>
+      <c r="E228">
+        <v>4.9310489999999998</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A229" s="2">
         <v>1097</v>
       </c>
@@ -2947,8 +4321,14 @@
       <c r="C229" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D229">
+        <v>52.345621999999999</v>
+      </c>
+      <c r="E229">
+        <v>4.9310489999999998</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A230" s="2">
         <v>1098</v>
       </c>
@@ -2957,6 +4337,12 @@
       </c>
       <c r="C230" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="D230">
+        <v>52.351914999999998</v>
+      </c>
+      <c r="E230">
+        <v>4.9477320000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>